<commit_message>
add structure of paper
</commit_message>
<xml_diff>
--- a/Data-new/countries.xlsx
+++ b/Data-new/countries.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{92A6A271-F623-41FA-BA5F-8CD2DC1D003B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{52CF1677-3D4D-46CE-A1CF-C080F1A25B08}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A8F7FD-BE16-478E-B12F-C359EC5BE27C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1156,9 +1156,6 @@
     <t>RU</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
     <t>RW</t>
   </si>
   <si>
@@ -1502,6 +1499,9 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>RUSSIAN FEDERATION</t>
   </si>
 </sst>
 </file>
@@ -1821,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:XFD73"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="D229" sqref="D229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3523,7 +3523,7 @@
         <v>127.76692199999999</v>
       </c>
       <c r="D121" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -4475,12 +4475,12 @@
         <v>105.31875599999999</v>
       </c>
       <c r="D189" t="s">
-        <v>378</v>
+        <v>493</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B190">
         <v>-1.9402779999999999</v>
@@ -4489,12 +4489,12 @@
         <v>29.873888000000001</v>
       </c>
       <c r="D190" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B191">
         <v>23.885942</v>
@@ -4503,12 +4503,12 @@
         <v>45.079161999999997</v>
       </c>
       <c r="D191" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B192">
         <v>-9.6457099999999993</v>
@@ -4517,12 +4517,12 @@
         <v>160.156194</v>
       </c>
       <c r="D192" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B193">
         <v>-4.6795739999999997</v>
@@ -4531,12 +4531,12 @@
         <v>55.491976999999999</v>
       </c>
       <c r="D193" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B194">
         <v>12.862807</v>
@@ -4545,12 +4545,12 @@
         <v>30.217635999999999</v>
       </c>
       <c r="D194" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B195">
         <v>60.128160999999999</v>
@@ -4559,12 +4559,12 @@
         <v>18.643501000000001</v>
       </c>
       <c r="D195" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B196">
         <v>1.3520829999999999</v>
@@ -4573,12 +4573,12 @@
         <v>103.819836</v>
       </c>
       <c r="D196" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B197">
         <v>-24.143474000000001</v>
@@ -4587,12 +4587,12 @@
         <v>-10.030696000000001</v>
       </c>
       <c r="D197" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B198">
         <v>46.151240999999999</v>
@@ -4601,12 +4601,12 @@
         <v>14.995463000000001</v>
       </c>
       <c r="D198" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B199">
         <v>77.553604000000007</v>
@@ -4615,12 +4615,12 @@
         <v>23.670272000000001</v>
       </c>
       <c r="D199" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B200">
         <v>48.669026000000002</v>
@@ -4629,12 +4629,12 @@
         <v>19.699024000000001</v>
       </c>
       <c r="D200" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B201">
         <v>8.4605549999999994</v>
@@ -4643,12 +4643,12 @@
         <v>-11.779889000000001</v>
       </c>
       <c r="D201" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B202">
         <v>43.942360000000001</v>
@@ -4657,12 +4657,12 @@
         <v>12.457777</v>
       </c>
       <c r="D202" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B203">
         <v>14.497401</v>
@@ -4671,12 +4671,12 @@
         <v>-14.452362000000001</v>
       </c>
       <c r="D203" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B204">
         <v>5.1521489999999996</v>
@@ -4685,12 +4685,12 @@
         <v>46.199615999999999</v>
       </c>
       <c r="D204" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B205">
         <v>3.919305</v>
@@ -4699,12 +4699,12 @@
         <v>-56.027782999999999</v>
       </c>
       <c r="D205" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B206">
         <v>0.18636</v>
@@ -4713,12 +4713,12 @@
         <v>6.6130810000000002</v>
       </c>
       <c r="D206" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B207">
         <v>13.794185000000001</v>
@@ -4727,12 +4727,12 @@
         <v>-88.896529999999998</v>
       </c>
       <c r="D207" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B208">
         <v>34.802075000000002</v>
@@ -4741,12 +4741,12 @@
         <v>38.996814999999998</v>
       </c>
       <c r="D208" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B209">
         <v>-26.522503</v>
@@ -4755,12 +4755,12 @@
         <v>31.465865999999998</v>
       </c>
       <c r="D209" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B210">
         <v>21.694025</v>
@@ -4769,12 +4769,12 @@
         <v>-71.797927999999999</v>
       </c>
       <c r="D210" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B211">
         <v>15.454166000000001</v>
@@ -4783,12 +4783,12 @@
         <v>18.732206999999999</v>
       </c>
       <c r="D211" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B212">
         <v>-49.280366000000001</v>
@@ -4797,12 +4797,12 @@
         <v>69.348557</v>
       </c>
       <c r="D212" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B213">
         <v>8.6195430000000002</v>
@@ -4811,12 +4811,12 @@
         <v>0.82478200000000002</v>
       </c>
       <c r="D213" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B214">
         <v>15.870032</v>
@@ -4825,12 +4825,12 @@
         <v>100.992541</v>
       </c>
       <c r="D214" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B215">
         <v>38.861033999999997</v>
@@ -4839,12 +4839,12 @@
         <v>71.276093000000003</v>
       </c>
       <c r="D215" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B216">
         <v>-8.9673630000000006</v>
@@ -4853,12 +4853,12 @@
         <v>-171.85588100000001</v>
       </c>
       <c r="D216" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B217">
         <v>-8.8742169999999998</v>
@@ -4867,12 +4867,12 @@
         <v>125.72753899999999</v>
       </c>
       <c r="D217" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B218">
         <v>38.969718999999998</v>
@@ -4881,12 +4881,12 @@
         <v>59.556277999999999</v>
       </c>
       <c r="D218" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B219">
         <v>33.886916999999997</v>
@@ -4895,12 +4895,12 @@
         <v>9.5374990000000004</v>
       </c>
       <c r="D219" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B220">
         <v>-21.178985999999998</v>
@@ -4909,12 +4909,12 @@
         <v>-175.19824199999999</v>
       </c>
       <c r="D220" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B221">
         <v>38.963745000000003</v>
@@ -4923,12 +4923,12 @@
         <v>35.243321999999999</v>
       </c>
       <c r="D221" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B222">
         <v>10.691803</v>
@@ -4937,12 +4937,12 @@
         <v>-61.222503000000003</v>
       </c>
       <c r="D222" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B223">
         <v>-7.1095350000000002</v>
@@ -4951,12 +4951,12 @@
         <v>177.64932999999999</v>
       </c>
       <c r="D223" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B224">
         <v>23.69781</v>
@@ -4965,12 +4965,12 @@
         <v>120.960515</v>
       </c>
       <c r="D224" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B225">
         <v>-6.3690280000000001</v>
@@ -4979,12 +4979,12 @@
         <v>34.888821999999998</v>
       </c>
       <c r="D225" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B226">
         <v>48.379432999999999</v>
@@ -4993,12 +4993,12 @@
         <v>31.165579999999999</v>
       </c>
       <c r="D226" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B227">
         <v>1.3733329999999999</v>
@@ -5007,20 +5007,20 @@
         <v>32.290275000000001</v>
       </c>
       <c r="D227" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
+        <v>454</v>
+      </c>
+      <c r="D228" t="s">
         <v>455</v>
-      </c>
-      <c r="D228" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B229">
         <v>37.090240000000001</v>
@@ -5029,12 +5029,12 @@
         <v>-95.712890999999999</v>
       </c>
       <c r="D229" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B230">
         <v>-32.522779</v>
@@ -5043,12 +5043,12 @@
         <v>-55.765835000000003</v>
       </c>
       <c r="D230" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B231">
         <v>41.377490999999999</v>
@@ -5057,12 +5057,12 @@
         <v>64.585262</v>
       </c>
       <c r="D231" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B232">
         <v>41.902915999999998</v>
@@ -5071,12 +5071,12 @@
         <v>12.453389</v>
       </c>
       <c r="D232" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B233">
         <v>12.984305000000001</v>
@@ -5085,12 +5085,12 @@
         <v>-61.287227999999999</v>
       </c>
       <c r="D233" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B234">
         <v>6.4237500000000001</v>
@@ -5099,12 +5099,12 @@
         <v>-66.589730000000003</v>
       </c>
       <c r="D234" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B235">
         <v>18.420694999999998</v>
@@ -5113,12 +5113,12 @@
         <v>-64.639967999999996</v>
       </c>
       <c r="D235" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B236">
         <v>18.335764999999999</v>
@@ -5127,12 +5127,12 @@
         <v>-64.896334999999993</v>
       </c>
       <c r="D236" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B237">
         <v>14.058324000000001</v>
@@ -5141,12 +5141,12 @@
         <v>108.277199</v>
       </c>
       <c r="D237" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B238">
         <v>-15.376706</v>
@@ -5155,12 +5155,12 @@
         <v>166.959158</v>
       </c>
       <c r="D238" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B239">
         <v>-13.768751999999999</v>
@@ -5169,12 +5169,12 @@
         <v>-177.15609699999999</v>
       </c>
       <c r="D239" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B240">
         <v>-13.759029</v>
@@ -5183,12 +5183,12 @@
         <v>-172.10462899999999</v>
       </c>
       <c r="D240" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B241">
         <v>42.602635999999997</v>
@@ -5197,12 +5197,12 @@
         <v>20.902977</v>
       </c>
       <c r="D241" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B242">
         <v>15.552727000000001</v>
@@ -5211,12 +5211,12 @@
         <v>48.516387999999999</v>
       </c>
       <c r="D242" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B243">
         <v>-12.827500000000001</v>
@@ -5225,12 +5225,12 @@
         <v>45.166243999999999</v>
       </c>
       <c r="D243" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B244">
         <v>-30.559481999999999</v>
@@ -5239,12 +5239,12 @@
         <v>22.937505999999999</v>
       </c>
       <c r="D244" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B245">
         <v>-13.133896999999999</v>
@@ -5253,12 +5253,12 @@
         <v>27.849332</v>
       </c>
       <c r="D245" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B246">
         <v>-19.015438</v>
@@ -5267,7 +5267,7 @@
         <v>29.154857</v>
       </c>
       <c r="D246" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>